<commit_message>
entry'lere varsayilan degerler atandi
</commit_message>
<xml_diff>
--- a/D3.xlsx
+++ b/D3.xlsx
@@ -5,13 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Sayfa1" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Sayfa2" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="Sayfa3" sheetId="3" state="visible" r:id="rId5"/>
-    <sheet name="Sayfa4" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="Sayfa2" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sayfa3" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Sayfa4" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Sayfa1" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -419,6 +419,75 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
     <tabColor rgb="FF00E676"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -513,38 +582,38 @@
       </c>
       <c r="I5" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="J5" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K5" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L5" s="12" t="str">
         <f aca="false">I5&amp;"."&amp;J5&amp;"."&amp;K5</f>
-        <v>4.3.2022</v>
+        <v>10.5.2022</v>
       </c>
       <c r="M5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>16329</v>
+        <v>6316</v>
       </c>
       <c r="N5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>22107</v>
+        <v>4017</v>
       </c>
       <c r="O5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>27178</v>
+        <v>4098</v>
       </c>
       <c r="P5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>3950</v>
+        <v>8806</v>
       </c>
       <c r="Q5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>22908</v>
+        <v>29067</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -572,34 +641,34 @@
       </c>
       <c r="J6" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K6" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L6" s="12" t="str">
         <f aca="false">I6&amp;"."&amp;J6&amp;"."&amp;K6</f>
-        <v>6.5.2022</v>
+        <v>6.7.2022</v>
       </c>
       <c r="M6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>10905</v>
+        <v>16377</v>
       </c>
       <c r="N6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>11302</v>
+        <v>29857</v>
       </c>
       <c r="O6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>14424</v>
+        <v>15164</v>
       </c>
       <c r="P6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>22881</v>
+        <v>28273</v>
       </c>
       <c r="Q6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>2459</v>
+        <v>4337</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -623,38 +692,38 @@
       </c>
       <c r="I7" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="J7" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="K7" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L7" s="12" t="str">
         <f aca="false">I7&amp;"."&amp;J7&amp;"."&amp;K7</f>
-        <v>7.11.2022</v>
+        <v>10.6.2022</v>
       </c>
       <c r="M7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>7083</v>
+        <v>17245</v>
       </c>
       <c r="N7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>7502</v>
+        <v>13859</v>
       </c>
       <c r="O7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>23813</v>
+        <v>20892</v>
       </c>
       <c r="P7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>5731</v>
+        <v>6114</v>
       </c>
       <c r="Q7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>10477</v>
+        <v>7815</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -678,38 +747,38 @@
       </c>
       <c r="I8" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J8" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="K8" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L8" s="12" t="str">
         <f aca="false">I8&amp;"."&amp;J8&amp;"."&amp;K8</f>
-        <v>9.4.2022</v>
+        <v>10.11.2022</v>
       </c>
       <c r="M8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>15234</v>
+        <v>18357</v>
       </c>
       <c r="N8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>9893</v>
+        <v>18155</v>
       </c>
       <c r="O8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>25997</v>
+        <v>11713</v>
       </c>
       <c r="P8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>17089</v>
+        <v>2533</v>
       </c>
       <c r="Q8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>789</v>
+        <v>7462</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -733,38 +802,38 @@
       </c>
       <c r="I9" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J9" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K9" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L9" s="12" t="str">
         <f aca="false">I9&amp;"."&amp;J9&amp;"."&amp;K9</f>
-        <v>5.3.2022</v>
+        <v>2.8.2022</v>
       </c>
       <c r="M9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>12826</v>
+        <v>21978</v>
       </c>
       <c r="N9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>19564</v>
+        <v>8439</v>
       </c>
       <c r="O9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>6534</v>
+        <v>29385</v>
       </c>
       <c r="P9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>22411</v>
+        <v>29879</v>
       </c>
       <c r="Q9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>21979</v>
+        <v>15405</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -788,38 +857,38 @@
       </c>
       <c r="I10" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="J10" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K10" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L10" s="12" t="str">
         <f aca="false">I10&amp;"."&amp;J10&amp;"."&amp;K10</f>
-        <v>10.3.2022</v>
+        <v>6.4.2022</v>
       </c>
       <c r="M10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>26599</v>
+        <v>19762</v>
       </c>
       <c r="N10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>15312</v>
+        <v>25661</v>
       </c>
       <c r="O10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>6473</v>
+        <v>13457</v>
       </c>
       <c r="P10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>10423</v>
+        <v>27025</v>
       </c>
       <c r="Q10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>28580</v>
+        <v>6463</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -847,34 +916,34 @@
       </c>
       <c r="J11" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="K11" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L11" s="12" t="str">
         <f aca="false">I11&amp;"."&amp;J11&amp;"."&amp;K11</f>
-        <v>6.11.2022</v>
+        <v>6.3.2022</v>
       </c>
       <c r="M11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>19346</v>
+        <v>9295</v>
       </c>
       <c r="N11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>28142</v>
+        <v>5583</v>
       </c>
       <c r="O11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>434</v>
+        <v>12841</v>
       </c>
       <c r="P11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>29383</v>
+        <v>1743</v>
       </c>
       <c r="Q11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>20089</v>
+        <v>15768</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1027,38 +1096,38 @@
       </c>
       <c r="I17" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="J17" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K17" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L17" s="12" t="str">
         <f aca="false">I17&amp;"."&amp;J17&amp;"."&amp;K17</f>
-        <v>3.2.2022</v>
+        <v>7.3.2022</v>
       </c>
       <c r="M17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>26463</v>
+        <v>28103</v>
       </c>
       <c r="N17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>19301</v>
+        <v>27212</v>
       </c>
       <c r="O17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>24852</v>
+        <v>25709</v>
       </c>
       <c r="P17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>26055</v>
+        <v>24468</v>
       </c>
       <c r="Q17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>27007</v>
+        <v>15991</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1082,7 +1151,7 @@
       </c>
       <c r="I18" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J18" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
@@ -1093,27 +1162,27 @@
       </c>
       <c r="L18" s="12" t="str">
         <f aca="false">I18&amp;"."&amp;J18&amp;"."&amp;K18</f>
-        <v>8.5.2022</v>
+        <v>6.5.2022</v>
       </c>
       <c r="M18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>19984</v>
+        <v>15724</v>
       </c>
       <c r="N18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>12891</v>
+        <v>7427</v>
       </c>
       <c r="O18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>28714</v>
+        <v>11969</v>
       </c>
       <c r="P18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>21783</v>
+        <v>14348</v>
       </c>
       <c r="Q18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>5469</v>
+        <v>29461</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1137,38 +1206,38 @@
       </c>
       <c r="I19" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J19" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="K19" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L19" s="12" t="str">
         <f aca="false">I19&amp;"."&amp;J19&amp;"."&amp;K19</f>
-        <v>9.11.2022</v>
+        <v>7.8.2022</v>
       </c>
       <c r="M19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>15240</v>
+        <v>20965</v>
       </c>
       <c r="N19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>6048</v>
+        <v>1770</v>
       </c>
       <c r="O19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>1850</v>
+        <v>23820</v>
       </c>
       <c r="P19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>16587</v>
+        <v>12977</v>
       </c>
       <c r="Q19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>23800</v>
+        <v>7239</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1192,38 +1261,38 @@
       </c>
       <c r="I20" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J20" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K20" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L20" s="12" t="str">
         <f aca="false">I20&amp;"."&amp;J20&amp;"."&amp;K20</f>
-        <v>1.6.2022</v>
+        <v>4.8.2022</v>
       </c>
       <c r="M20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>2307</v>
+        <v>19638</v>
       </c>
       <c r="N20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>16537</v>
+        <v>10433</v>
       </c>
       <c r="O20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>7403</v>
+        <v>29356</v>
       </c>
       <c r="P20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>10045</v>
+        <v>28196</v>
       </c>
       <c r="Q20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>23635</v>
+        <v>13451</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1247,38 +1316,38 @@
       </c>
       <c r="I21" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J21" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="K21" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L21" s="12" t="str">
         <f aca="false">I21&amp;"."&amp;J21&amp;"."&amp;K21</f>
-        <v>3.9.2022</v>
+        <v>1.11.2022</v>
       </c>
       <c r="M21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>26075</v>
+        <v>16998</v>
       </c>
       <c r="N21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>16489</v>
+        <v>1036</v>
       </c>
       <c r="O21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>14926</v>
+        <v>13022</v>
       </c>
       <c r="P21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>20952</v>
+        <v>10837</v>
       </c>
       <c r="Q21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>25745</v>
+        <v>820</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1302,38 +1371,38 @@
       </c>
       <c r="I22" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J22" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="K22" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L22" s="12" t="str">
         <f aca="false">I22&amp;"."&amp;J22&amp;"."&amp;K22</f>
-        <v>1.7.2022</v>
+        <v>6.2.2022</v>
       </c>
       <c r="M22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>17134</v>
+        <v>15666</v>
       </c>
       <c r="N22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>18663</v>
+        <v>7327</v>
       </c>
       <c r="O22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>22441</v>
+        <v>3306</v>
       </c>
       <c r="P22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>23283</v>
+        <v>27840</v>
       </c>
       <c r="Q22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>10011</v>
+        <v>25720</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1357,38 +1426,38 @@
       </c>
       <c r="I23" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="J23" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K23" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L23" s="12" t="str">
         <f aca="false">I23&amp;"."&amp;J23&amp;"."&amp;K23</f>
-        <v>6.8.2022</v>
+        <v>9.10.2022</v>
       </c>
       <c r="M23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>7032</v>
+        <v>5736</v>
       </c>
       <c r="N23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>2592</v>
+        <v>14724</v>
       </c>
       <c r="O23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>29620</v>
+        <v>16337</v>
       </c>
       <c r="P23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>26359</v>
+        <v>3315</v>
       </c>
       <c r="Q23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>27900</v>
+        <v>257</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1541,38 +1610,38 @@
       </c>
       <c r="I29" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J29" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="K29" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L29" s="12" t="str">
         <f aca="false">I29&amp;"."&amp;J29&amp;"."&amp;K29</f>
-        <v>3.11.2022</v>
+        <v>2.2.2022</v>
       </c>
       <c r="M29" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>20630</v>
+        <v>26429</v>
       </c>
       <c r="N29" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>12015</v>
+        <v>10008</v>
       </c>
       <c r="O29" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>27975</v>
+        <v>498</v>
       </c>
       <c r="P29" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>22634</v>
+        <v>27534</v>
       </c>
       <c r="Q29" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>25326</v>
+        <v>927</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1596,38 +1665,38 @@
       </c>
       <c r="I30" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="J30" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="K30" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L30" s="12" t="str">
         <f aca="false">I30&amp;"."&amp;J30&amp;"."&amp;K30</f>
-        <v>2.8.2022</v>
+        <v>9.11.2022</v>
       </c>
       <c r="M30" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>26039</v>
+        <v>13088</v>
       </c>
       <c r="N30" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>22059</v>
+        <v>4960</v>
       </c>
       <c r="O30" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>24028</v>
+        <v>11593</v>
       </c>
       <c r="P30" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>1594</v>
+        <v>11871</v>
       </c>
       <c r="Q30" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>9170</v>
+        <v>26886</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1651,38 +1720,38 @@
       </c>
       <c r="I31" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J31" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="K31" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L31" s="12" t="str">
         <f aca="false">I31&amp;"."&amp;J31&amp;"."&amp;K31</f>
-        <v>6.10.2022</v>
+        <v>8.6.2022</v>
       </c>
       <c r="M31" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>23525</v>
+        <v>19898</v>
       </c>
       <c r="N31" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>19183</v>
+        <v>20626</v>
       </c>
       <c r="O31" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>26891</v>
+        <v>22464</v>
       </c>
       <c r="P31" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>17603</v>
+        <v>27491</v>
       </c>
       <c r="Q31" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>16716</v>
+        <v>16807</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1706,38 +1775,38 @@
       </c>
       <c r="I32" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J32" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K32" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L32" s="12" t="str">
         <f aca="false">I32&amp;"."&amp;J32&amp;"."&amp;K32</f>
-        <v>2.2.2022</v>
+        <v>3.6.2022</v>
       </c>
       <c r="M32" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>11997</v>
+        <v>9463</v>
       </c>
       <c r="N32" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>1415</v>
+        <v>16318</v>
       </c>
       <c r="O32" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>25893</v>
+        <v>20307</v>
       </c>
       <c r="P32" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>28799</v>
+        <v>19663</v>
       </c>
       <c r="Q32" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>17192</v>
+        <v>27459</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1761,38 +1830,38 @@
       </c>
       <c r="I33" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="J33" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="K33" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L33" s="12" t="str">
         <f aca="false">I33&amp;"."&amp;J33&amp;"."&amp;K33</f>
-        <v>9.4.2022</v>
+        <v>2.10.2022</v>
       </c>
       <c r="M33" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>12011</v>
+        <v>15332</v>
       </c>
       <c r="N33" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>5116</v>
+        <v>5043</v>
       </c>
       <c r="O33" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>24863</v>
+        <v>4269</v>
       </c>
       <c r="P33" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>16829</v>
+        <v>10276</v>
       </c>
       <c r="Q33" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>8572</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1816,38 +1885,38 @@
       </c>
       <c r="I34" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J34" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K34" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L34" s="12" t="str">
         <f aca="false">I34&amp;"."&amp;J34&amp;"."&amp;K34</f>
-        <v>10.3.2022</v>
+        <v>9.7.2022</v>
       </c>
       <c r="M34" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>1891</v>
+        <v>14880</v>
       </c>
       <c r="N34" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>28537</v>
+        <v>17069</v>
       </c>
       <c r="O34" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>8030</v>
+        <v>22695</v>
       </c>
       <c r="P34" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>10353</v>
+        <v>547</v>
       </c>
       <c r="Q34" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>3192</v>
+        <v>3905</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1871,38 +1940,38 @@
       </c>
       <c r="I35" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J35" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K35" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L35" s="12" t="str">
         <f aca="false">I35&amp;"."&amp;J35&amp;"."&amp;K35</f>
-        <v>3.10.2022</v>
+        <v>2.9.2022</v>
       </c>
       <c r="M35" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>10501</v>
+        <v>16236</v>
       </c>
       <c r="N35" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>10823</v>
+        <v>17314</v>
       </c>
       <c r="O35" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>5076</v>
+        <v>28868</v>
       </c>
       <c r="P35" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>9650</v>
+        <v>10149</v>
       </c>
       <c r="Q35" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>5321</v>
+        <v>615</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2034,73 +2103,4 @@
     <oddFooter>&amp;CSayfa &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
duzgun calisan ilk kodlar
</commit_message>
<xml_diff>
--- a/D3.xlsx
+++ b/D3.xlsx
@@ -582,38 +582,38 @@
       </c>
       <c r="I5" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="J5" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="K5" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L5" s="12" t="str">
         <f aca="false">I5&amp;"."&amp;J5&amp;"."&amp;K5</f>
-        <v>10.5.2022</v>
+        <v>7.8.2022</v>
       </c>
       <c r="M5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>6316</v>
+        <v>2409</v>
       </c>
       <c r="N5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>4017</v>
+        <v>22257</v>
       </c>
       <c r="O5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>4098</v>
+        <v>4972</v>
       </c>
       <c r="P5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>8806</v>
+        <v>19343</v>
       </c>
       <c r="Q5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>29067</v>
+        <v>15458</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -637,38 +637,38 @@
       </c>
       <c r="I6" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J6" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K6" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L6" s="12" t="str">
         <f aca="false">I6&amp;"."&amp;J6&amp;"."&amp;K6</f>
-        <v>6.7.2022</v>
+        <v>8.3.2022</v>
       </c>
       <c r="M6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>16377</v>
+        <v>24465</v>
       </c>
       <c r="N6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>29857</v>
+        <v>1752</v>
       </c>
       <c r="O6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>15164</v>
+        <v>7577</v>
       </c>
       <c r="P6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>28273</v>
+        <v>4169</v>
       </c>
       <c r="Q6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>4337</v>
+        <v>20382</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -692,38 +692,38 @@
       </c>
       <c r="I7" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J7" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K7" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L7" s="12" t="str">
         <f aca="false">I7&amp;"."&amp;J7&amp;"."&amp;K7</f>
-        <v>10.6.2022</v>
+        <v>8.2.2022</v>
       </c>
       <c r="M7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>17245</v>
+        <v>27683</v>
       </c>
       <c r="N7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>13859</v>
+        <v>21256</v>
       </c>
       <c r="O7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>20892</v>
+        <v>23721</v>
       </c>
       <c r="P7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>6114</v>
+        <v>1694</v>
       </c>
       <c r="Q7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>7815</v>
+        <v>24132</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -747,38 +747,38 @@
       </c>
       <c r="I8" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="J8" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="K8" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L8" s="12" t="str">
         <f aca="false">I8&amp;"."&amp;J8&amp;"."&amp;K8</f>
-        <v>10.11.2022</v>
+        <v>2.8.2022</v>
       </c>
       <c r="M8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>18357</v>
+        <v>8715</v>
       </c>
       <c r="N8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>18155</v>
+        <v>29454</v>
       </c>
       <c r="O8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>11713</v>
+        <v>18021</v>
       </c>
       <c r="P8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>2533</v>
+        <v>16471</v>
       </c>
       <c r="Q8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>7462</v>
+        <v>20489</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -802,38 +802,38 @@
       </c>
       <c r="I9" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J9" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K9" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L9" s="12" t="str">
         <f aca="false">I9&amp;"."&amp;J9&amp;"."&amp;K9</f>
-        <v>2.8.2022</v>
+        <v>1.10.2022</v>
       </c>
       <c r="M9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>21978</v>
+        <v>14289</v>
       </c>
       <c r="N9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>8439</v>
+        <v>28395</v>
       </c>
       <c r="O9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>29385</v>
+        <v>1159</v>
       </c>
       <c r="P9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>29879</v>
+        <v>16711</v>
       </c>
       <c r="Q9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>15405</v>
+        <v>16242</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -857,38 +857,38 @@
       </c>
       <c r="I10" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J10" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="K10" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L10" s="12" t="str">
         <f aca="false">I10&amp;"."&amp;J10&amp;"."&amp;K10</f>
-        <v>6.4.2022</v>
+        <v>7.12.2022</v>
       </c>
       <c r="M10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>19762</v>
+        <v>16002</v>
       </c>
       <c r="N10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>25661</v>
+        <v>6278</v>
       </c>
       <c r="O10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>13457</v>
+        <v>5660</v>
       </c>
       <c r="P10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>27025</v>
+        <v>2080</v>
       </c>
       <c r="Q10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>6463</v>
+        <v>8770</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -916,34 +916,34 @@
       </c>
       <c r="J11" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="K11" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L11" s="12" t="str">
         <f aca="false">I11&amp;"."&amp;J11&amp;"."&amp;K11</f>
-        <v>6.3.2022</v>
+        <v>6.12.2022</v>
       </c>
       <c r="M11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>9295</v>
+        <v>4377</v>
       </c>
       <c r="N11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>5583</v>
+        <v>24250</v>
       </c>
       <c r="O11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>12841</v>
+        <v>4331</v>
       </c>
       <c r="P11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>1743</v>
+        <v>6492</v>
       </c>
       <c r="Q11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>15768</v>
+        <v>18514</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1096,38 +1096,38 @@
       </c>
       <c r="I17" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J17" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K17" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L17" s="12" t="str">
         <f aca="false">I17&amp;"."&amp;J17&amp;"."&amp;K17</f>
-        <v>7.3.2022</v>
+        <v>9.6.2022</v>
       </c>
       <c r="M17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>28103</v>
+        <v>19762</v>
       </c>
       <c r="N17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>27212</v>
+        <v>28093</v>
       </c>
       <c r="O17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>25709</v>
+        <v>13720</v>
       </c>
       <c r="P17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>24468</v>
+        <v>24290</v>
       </c>
       <c r="Q17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>15991</v>
+        <v>24270</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1151,38 +1151,38 @@
       </c>
       <c r="I18" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J18" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="K18" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L18" s="12" t="str">
         <f aca="false">I18&amp;"."&amp;J18&amp;"."&amp;K18</f>
-        <v>6.5.2022</v>
+        <v>2.12.2022</v>
       </c>
       <c r="M18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>15724</v>
+        <v>14016</v>
       </c>
       <c r="N18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>7427</v>
+        <v>444</v>
       </c>
       <c r="O18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>11969</v>
+        <v>5710</v>
       </c>
       <c r="P18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>14348</v>
+        <v>27833</v>
       </c>
       <c r="Q18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>29461</v>
+        <v>17313</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1206,38 +1206,38 @@
       </c>
       <c r="I19" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="J19" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="K19" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L19" s="12" t="str">
         <f aca="false">I19&amp;"."&amp;J19&amp;"."&amp;K19</f>
-        <v>7.8.2022</v>
+        <v>2.5.2022</v>
       </c>
       <c r="M19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>20965</v>
+        <v>15597</v>
       </c>
       <c r="N19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>1770</v>
+        <v>649</v>
       </c>
       <c r="O19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>23820</v>
+        <v>242</v>
       </c>
       <c r="P19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>12977</v>
+        <v>4884</v>
       </c>
       <c r="Q19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>7239</v>
+        <v>28596</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1261,38 +1261,38 @@
       </c>
       <c r="I20" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="J20" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="K20" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L20" s="12" t="str">
         <f aca="false">I20&amp;"."&amp;J20&amp;"."&amp;K20</f>
-        <v>4.8.2022</v>
+        <v>9.12.2022</v>
       </c>
       <c r="M20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>19638</v>
+        <v>14773</v>
       </c>
       <c r="N20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>10433</v>
+        <v>11865</v>
       </c>
       <c r="O20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>29356</v>
+        <v>15919</v>
       </c>
       <c r="P20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>28196</v>
+        <v>25273</v>
       </c>
       <c r="Q20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>13451</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1316,38 +1316,38 @@
       </c>
       <c r="I21" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J21" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="K21" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L21" s="12" t="str">
         <f aca="false">I21&amp;"."&amp;J21&amp;"."&amp;K21</f>
-        <v>1.11.2022</v>
+        <v>10.4.2022</v>
       </c>
       <c r="M21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>16998</v>
+        <v>12353</v>
       </c>
       <c r="N21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>1036</v>
+        <v>20459</v>
       </c>
       <c r="O21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>13022</v>
+        <v>17999</v>
       </c>
       <c r="P21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>10837</v>
+        <v>15240</v>
       </c>
       <c r="Q21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>820</v>
+        <v>28995</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1371,7 +1371,7 @@
       </c>
       <c r="I22" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J22" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
@@ -1382,27 +1382,27 @@
       </c>
       <c r="L22" s="12" t="str">
         <f aca="false">I22&amp;"."&amp;J22&amp;"."&amp;K22</f>
-        <v>6.2.2022</v>
+        <v>8.2.2022</v>
       </c>
       <c r="M22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>15666</v>
+        <v>25469</v>
       </c>
       <c r="N22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>7327</v>
+        <v>889</v>
       </c>
       <c r="O22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>3306</v>
+        <v>27346</v>
       </c>
       <c r="P22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>27840</v>
+        <v>12413</v>
       </c>
       <c r="Q22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>25720</v>
+        <v>11712</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1426,38 +1426,38 @@
       </c>
       <c r="I23" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J23" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K23" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L23" s="12" t="str">
         <f aca="false">I23&amp;"."&amp;J23&amp;"."&amp;K23</f>
-        <v>9.10.2022</v>
+        <v>7.8.2022</v>
       </c>
       <c r="M23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>5736</v>
+        <v>15857</v>
       </c>
       <c r="N23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>14724</v>
+        <v>18778</v>
       </c>
       <c r="O23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>16337</v>
+        <v>15282</v>
       </c>
       <c r="P23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>3315</v>
+        <v>14821</v>
       </c>
       <c r="Q23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>257</v>
+        <v>12682</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1610,38 +1610,38 @@
       </c>
       <c r="I29" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J29" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K29" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L29" s="12" t="str">
         <f aca="false">I29&amp;"."&amp;J29&amp;"."&amp;K29</f>
-        <v>2.2.2022</v>
+        <v>3.4.2022</v>
       </c>
       <c r="M29" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>26429</v>
+        <v>4122</v>
       </c>
       <c r="N29" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>10008</v>
+        <v>18004</v>
       </c>
       <c r="O29" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>498</v>
+        <v>18130</v>
       </c>
       <c r="P29" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>27534</v>
+        <v>276</v>
       </c>
       <c r="Q29" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>927</v>
+        <v>10672</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1665,38 +1665,38 @@
       </c>
       <c r="I30" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="J30" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="K30" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L30" s="12" t="str">
         <f aca="false">I30&amp;"."&amp;J30&amp;"."&amp;K30</f>
-        <v>9.11.2022</v>
+        <v>1.1.2022</v>
       </c>
       <c r="M30" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>13088</v>
+        <v>25395</v>
       </c>
       <c r="N30" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>4960</v>
+        <v>25258</v>
       </c>
       <c r="O30" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>11593</v>
+        <v>20675</v>
       </c>
       <c r="P30" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>11871</v>
+        <v>26246</v>
       </c>
       <c r="Q30" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>26886</v>
+        <v>25999</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1720,38 +1720,38 @@
       </c>
       <c r="I31" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J31" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K31" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L31" s="12" t="str">
         <f aca="false">I31&amp;"."&amp;J31&amp;"."&amp;K31</f>
-        <v>8.6.2022</v>
+        <v>6.1.2022</v>
       </c>
       <c r="M31" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>19898</v>
+        <v>10901</v>
       </c>
       <c r="N31" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>20626</v>
+        <v>15777</v>
       </c>
       <c r="O31" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>22464</v>
+        <v>6899</v>
       </c>
       <c r="P31" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>27491</v>
+        <v>10627</v>
       </c>
       <c r="Q31" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>16807</v>
+        <v>16483</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1775,38 +1775,38 @@
       </c>
       <c r="I32" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J32" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K32" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L32" s="12" t="str">
         <f aca="false">I32&amp;"."&amp;J32&amp;"."&amp;K32</f>
-        <v>3.6.2022</v>
+        <v>5.7.2022</v>
       </c>
       <c r="M32" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>9463</v>
+        <v>28781</v>
       </c>
       <c r="N32" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>16318</v>
+        <v>10243</v>
       </c>
       <c r="O32" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>20307</v>
+        <v>4401</v>
       </c>
       <c r="P32" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>19663</v>
+        <v>29427</v>
       </c>
       <c r="Q32" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>27459</v>
+        <v>21558</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1830,38 +1830,38 @@
       </c>
       <c r="I33" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J33" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="K33" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L33" s="12" t="str">
         <f aca="false">I33&amp;"."&amp;J33&amp;"."&amp;K33</f>
-        <v>2.10.2022</v>
+        <v>3.3.2022</v>
       </c>
       <c r="M33" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>15332</v>
+        <v>21204</v>
       </c>
       <c r="N33" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>5043</v>
+        <v>9872</v>
       </c>
       <c r="O33" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>4269</v>
+        <v>17517</v>
       </c>
       <c r="P33" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>10276</v>
+        <v>17704</v>
       </c>
       <c r="Q33" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>4000</v>
+        <v>8163</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1885,38 +1885,38 @@
       </c>
       <c r="I34" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="J34" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K34" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L34" s="12" t="str">
         <f aca="false">I34&amp;"."&amp;J34&amp;"."&amp;K34</f>
-        <v>9.7.2022</v>
+        <v>1.8.2022</v>
       </c>
       <c r="M34" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>14880</v>
+        <v>5939</v>
       </c>
       <c r="N34" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>17069</v>
+        <v>3946</v>
       </c>
       <c r="O34" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>22695</v>
+        <v>12678</v>
       </c>
       <c r="P34" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>547</v>
+        <v>22780</v>
       </c>
       <c r="Q34" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>3905</v>
+        <v>18881</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1940,38 +1940,38 @@
       </c>
       <c r="I35" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J35" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="K35" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L35" s="12" t="str">
         <f aca="false">I35&amp;"."&amp;J35&amp;"."&amp;K35</f>
-        <v>2.9.2022</v>
+        <v>6.7.2022</v>
       </c>
       <c r="M35" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>16236</v>
+        <v>19737</v>
       </c>
       <c r="N35" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>17314</v>
+        <v>9828</v>
       </c>
       <c r="O35" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>28868</v>
+        <v>23859</v>
       </c>
       <c r="P35" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>10149</v>
+        <v>19391</v>
       </c>
       <c r="Q35" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>615</v>
+        <v>574</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
kademe kademe ilerleme basladi
</commit_message>
<xml_diff>
--- a/D3.xlsx
+++ b/D3.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sayfa-1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="syf1" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="Sayfa2" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="Sayfa3" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="Sayfa4" sheetId="4" state="visible" r:id="rId6"/>
@@ -512,38 +512,38 @@
       </c>
       <c r="I5" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J5" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="K5" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L5" s="12" t="str">
         <f aca="false">I5&amp;"."&amp;J5&amp;"."&amp;K5</f>
-        <v>8.7.2022</v>
+        <v>10.11.2022</v>
       </c>
       <c r="M5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>9900</v>
+        <v>26142</v>
       </c>
       <c r="N5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>26664</v>
+        <v>2744</v>
       </c>
       <c r="O5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>7078</v>
+        <v>14144</v>
       </c>
       <c r="P5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>26507</v>
+        <v>7994</v>
       </c>
       <c r="Q5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>9163</v>
+        <v>4211</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -567,38 +567,38 @@
       </c>
       <c r="I6" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J6" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="K6" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L6" s="12" t="str">
         <f aca="false">I6&amp;"."&amp;J6&amp;"."&amp;K6</f>
-        <v>10.6.2022</v>
+        <v>5.11.2022</v>
       </c>
       <c r="M6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>2832</v>
+        <v>21346</v>
       </c>
       <c r="N6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>22684</v>
+        <v>5584</v>
       </c>
       <c r="O6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>28809</v>
+        <v>22944</v>
       </c>
       <c r="P6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>13725</v>
+        <v>402</v>
       </c>
       <c r="Q6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>637</v>
+        <v>1857</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -622,38 +622,38 @@
       </c>
       <c r="I7" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J7" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="K7" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L7" s="12" t="str">
         <f aca="false">I7&amp;"."&amp;J7&amp;"."&amp;K7</f>
-        <v>1.10.2022</v>
+        <v>2.4.2022</v>
       </c>
       <c r="M7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>24224</v>
+        <v>8555</v>
       </c>
       <c r="N7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>22081</v>
+        <v>8937</v>
       </c>
       <c r="O7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>17291</v>
+        <v>23279</v>
       </c>
       <c r="P7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>2251</v>
+        <v>27830</v>
       </c>
       <c r="Q7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>5795</v>
+        <v>3713</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -677,38 +677,38 @@
       </c>
       <c r="I8" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J8" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="K8" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L8" s="12" t="str">
         <f aca="false">I8&amp;"."&amp;J8&amp;"."&amp;K8</f>
-        <v>6.9.2022</v>
+        <v>7.3.2022</v>
       </c>
       <c r="M8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>26881</v>
+        <v>2906</v>
       </c>
       <c r="N8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>12750</v>
+        <v>5180</v>
       </c>
       <c r="O8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>17960</v>
+        <v>6719</v>
       </c>
       <c r="P8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>22540</v>
+        <v>7291</v>
       </c>
       <c r="Q8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>11292</v>
+        <v>18990</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -732,38 +732,38 @@
       </c>
       <c r="I9" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J9" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K9" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L9" s="12" t="str">
         <f aca="false">I9&amp;"."&amp;J9&amp;"."&amp;K9</f>
-        <v>1.11.2022</v>
+        <v>10.9.2022</v>
       </c>
       <c r="M9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>18615</v>
+        <v>21990</v>
       </c>
       <c r="N9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>565</v>
+        <v>13477</v>
       </c>
       <c r="O9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>28478</v>
+        <v>5040</v>
       </c>
       <c r="P9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>13492</v>
+        <v>25427</v>
       </c>
       <c r="Q9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>17931</v>
+        <v>10032</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -787,38 +787,38 @@
       </c>
       <c r="I10" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="J10" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="K10" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L10" s="12" t="str">
         <f aca="false">I10&amp;"."&amp;J10&amp;"."&amp;K10</f>
-        <v>3.12.2022</v>
+        <v>9.4.2022</v>
       </c>
       <c r="M10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>10255</v>
+        <v>27013</v>
       </c>
       <c r="N10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>22697</v>
+        <v>7206</v>
       </c>
       <c r="O10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>5386</v>
+        <v>2395</v>
       </c>
       <c r="P10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>5795</v>
+        <v>3014</v>
       </c>
       <c r="Q10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>18332</v>
+        <v>9002</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -842,38 +842,38 @@
       </c>
       <c r="I11" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J11" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="K11" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L11" s="12" t="str">
         <f aca="false">I11&amp;"."&amp;J11&amp;"."&amp;K11</f>
-        <v>3.2.2022</v>
+        <v>1.7.2022</v>
       </c>
       <c r="M11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>22533</v>
+        <v>9398</v>
       </c>
       <c r="N11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>21556</v>
+        <v>19907</v>
       </c>
       <c r="O11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>22181</v>
+        <v>441</v>
       </c>
       <c r="P11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>21999</v>
+        <v>12336</v>
       </c>
       <c r="Q11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>3962</v>
+        <v>12931</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1026,38 +1026,38 @@
       </c>
       <c r="I17" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J17" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K17" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L17" s="12" t="str">
         <f aca="false">I17&amp;"."&amp;J17&amp;"."&amp;K17</f>
-        <v>6.5.2022</v>
+        <v>8.3.2022</v>
       </c>
       <c r="M17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>16890</v>
+        <v>13421</v>
       </c>
       <c r="N17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>21376</v>
+        <v>17858</v>
       </c>
       <c r="O17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>4677</v>
+        <v>16526</v>
       </c>
       <c r="P17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>18152</v>
+        <v>1939</v>
       </c>
       <c r="Q17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>15701</v>
+        <v>26411</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1081,38 +1081,38 @@
       </c>
       <c r="I18" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J18" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="K18" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L18" s="12" t="str">
         <f aca="false">I18&amp;"."&amp;J18&amp;"."&amp;K18</f>
-        <v>2.11.2022</v>
+        <v>6.8.2022</v>
       </c>
       <c r="M18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>16709</v>
+        <v>14942</v>
       </c>
       <c r="N18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>3979</v>
+        <v>25968</v>
       </c>
       <c r="O18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>3290</v>
+        <v>10547</v>
       </c>
       <c r="P18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>22520</v>
+        <v>10019</v>
       </c>
       <c r="Q18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>15538</v>
+        <v>5697</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1136,38 +1136,38 @@
       </c>
       <c r="I19" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="J19" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K19" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L19" s="12" t="str">
         <f aca="false">I19&amp;"."&amp;J19&amp;"."&amp;K19</f>
-        <v>8.2.2022</v>
+        <v>3.5.2022</v>
       </c>
       <c r="M19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>6292</v>
+        <v>8109</v>
       </c>
       <c r="N19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>28241</v>
+        <v>4028</v>
       </c>
       <c r="O19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>6356</v>
+        <v>26381</v>
       </c>
       <c r="P19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>6758</v>
+        <v>26152</v>
       </c>
       <c r="Q19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>3009</v>
+        <v>11598</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1191,38 +1191,38 @@
       </c>
       <c r="I20" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J20" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K20" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L20" s="12" t="str">
         <f aca="false">I20&amp;"."&amp;J20&amp;"."&amp;K20</f>
-        <v>6.2.2022</v>
+        <v>5.5.2022</v>
       </c>
       <c r="M20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>29995</v>
+        <v>11529</v>
       </c>
       <c r="N20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>16058</v>
+        <v>4863</v>
       </c>
       <c r="O20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>2063</v>
+        <v>2648</v>
       </c>
       <c r="P20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>19434</v>
+        <v>2404</v>
       </c>
       <c r="Q20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>165</v>
+        <v>12277</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1246,38 +1246,38 @@
       </c>
       <c r="I21" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="J21" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="K21" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L21" s="12" t="str">
         <f aca="false">I21&amp;"."&amp;J21&amp;"."&amp;K21</f>
-        <v>3.10.2022</v>
+        <v>10.1.2022</v>
       </c>
       <c r="M21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>4224</v>
+        <v>28630</v>
       </c>
       <c r="N21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>24791</v>
+        <v>20537</v>
       </c>
       <c r="O21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>17275</v>
+        <v>569</v>
       </c>
       <c r="P21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>11205</v>
+        <v>19954</v>
       </c>
       <c r="Q21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>5707</v>
+        <v>828</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1301,38 +1301,38 @@
       </c>
       <c r="I22" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J22" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="K22" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L22" s="12" t="str">
         <f aca="false">I22&amp;"."&amp;J22&amp;"."&amp;K22</f>
-        <v>8.11.2022</v>
+        <v>10.7.2022</v>
       </c>
       <c r="M22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>25675</v>
+        <v>6844</v>
       </c>
       <c r="N22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>22094</v>
+        <v>7071</v>
       </c>
       <c r="O22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>23616</v>
+        <v>15777</v>
       </c>
       <c r="P22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>19069</v>
+        <v>29728</v>
       </c>
       <c r="Q22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>8051</v>
+        <v>3968</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1356,38 +1356,38 @@
       </c>
       <c r="I23" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="J23" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="K23" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L23" s="12" t="str">
         <f aca="false">I23&amp;"."&amp;J23&amp;"."&amp;K23</f>
-        <v>10.8.2022</v>
+        <v>4.11.2022</v>
       </c>
       <c r="M23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>29677</v>
+        <v>4024</v>
       </c>
       <c r="N23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>6606</v>
+        <v>5535</v>
       </c>
       <c r="O23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>12239</v>
+        <v>27308</v>
       </c>
       <c r="P23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>21838</v>
+        <v>20294</v>
       </c>
       <c r="Q23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>19396</v>
+        <v>2284</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1540,38 +1540,38 @@
       </c>
       <c r="I29" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J29" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="K29" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L29" s="12" t="str">
         <f aca="false">I29&amp;"."&amp;J29&amp;"."&amp;K29</f>
-        <v>3.8.2022</v>
+        <v>4.3.2022</v>
       </c>
       <c r="M29" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>4779</v>
+        <v>29493</v>
       </c>
       <c r="N29" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>14506</v>
+        <v>21760</v>
       </c>
       <c r="O29" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>10319</v>
+        <v>26794</v>
       </c>
       <c r="P29" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>16935</v>
+        <v>21631</v>
       </c>
       <c r="Q29" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>12640</v>
+        <v>9671</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1599,34 +1599,34 @@
       </c>
       <c r="J30" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K30" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L30" s="12" t="str">
         <f aca="false">I30&amp;"."&amp;J30&amp;"."&amp;K30</f>
-        <v>5.6.2022</v>
+        <v>5.2.2022</v>
       </c>
       <c r="M30" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>9448</v>
+        <v>6645</v>
       </c>
       <c r="N30" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>20906</v>
+        <v>1844</v>
       </c>
       <c r="O30" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>21413</v>
+        <v>14526</v>
       </c>
       <c r="P30" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>20320</v>
+        <v>22780</v>
       </c>
       <c r="Q30" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>12425</v>
+        <v>23471</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1650,38 +1650,38 @@
       </c>
       <c r="I31" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="J31" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="K31" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L31" s="12" t="str">
         <f aca="false">I31&amp;"."&amp;J31&amp;"."&amp;K31</f>
-        <v>3.9.2022</v>
+        <v>8.4.2022</v>
       </c>
       <c r="M31" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>11877</v>
+        <v>4968</v>
       </c>
       <c r="N31" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>24091</v>
+        <v>23345</v>
       </c>
       <c r="O31" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>1205</v>
+        <v>7174</v>
       </c>
       <c r="P31" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>15939</v>
+        <v>14181</v>
       </c>
       <c r="Q31" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>18537</v>
+        <v>14242</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1705,38 +1705,38 @@
       </c>
       <c r="I32" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J32" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="K32" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L32" s="12" t="str">
         <f aca="false">I32&amp;"."&amp;J32&amp;"."&amp;K32</f>
-        <v>4.2.2022</v>
+        <v>5.11.2022</v>
       </c>
       <c r="M32" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>7935</v>
+        <v>19214</v>
       </c>
       <c r="N32" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>8515</v>
+        <v>4027</v>
       </c>
       <c r="O32" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>6577</v>
+        <v>4485</v>
       </c>
       <c r="P32" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>18056</v>
+        <v>9290</v>
       </c>
       <c r="Q32" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>22631</v>
+        <v>5225</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1764,34 +1764,34 @@
       </c>
       <c r="J33" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="K33" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L33" s="12" t="str">
         <f aca="false">I33&amp;"."&amp;J33&amp;"."&amp;K33</f>
-        <v>2.11.2022</v>
+        <v>2.7.2022</v>
       </c>
       <c r="M33" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>1522</v>
+        <v>21617</v>
       </c>
       <c r="N33" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>22102</v>
+        <v>25050</v>
       </c>
       <c r="O33" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>1319</v>
+        <v>21447</v>
       </c>
       <c r="P33" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>19117</v>
+        <v>583</v>
       </c>
       <c r="Q33" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>957</v>
+        <v>19493</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1815,7 +1815,7 @@
       </c>
       <c r="I34" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J34" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
@@ -1826,27 +1826,27 @@
       </c>
       <c r="L34" s="12" t="str">
         <f aca="false">I34&amp;"."&amp;J34&amp;"."&amp;K34</f>
-        <v>2.5.2022</v>
+        <v>1.5.2022</v>
       </c>
       <c r="M34" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>6252</v>
+        <v>14043</v>
       </c>
       <c r="N34" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>17957</v>
+        <v>1963</v>
       </c>
       <c r="O34" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>21104</v>
+        <v>11326</v>
       </c>
       <c r="P34" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>8304</v>
+        <v>10431</v>
       </c>
       <c r="Q34" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>17766</v>
+        <v>15112</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1885,23 +1885,23 @@
       </c>
       <c r="M35" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>28766</v>
+        <v>18482</v>
       </c>
       <c r="N35" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>20465</v>
+        <v>4211</v>
       </c>
       <c r="O35" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>7035</v>
+        <v>26691</v>
       </c>
       <c r="P35" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>15100</v>
+        <v>6619</v>
       </c>
       <c r="Q35" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>9527</v>
+        <v>22048</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
baslik fonk.'a "try/except" blogu eklendi
</commit_message>
<xml_diff>
--- a/D3.xlsx
+++ b/D3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="syf1" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Sayfa2" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="Sayfa3" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Sayfa2" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sayfa3" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="syf1" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="Sayfa4" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -418,13 +418,59 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
     <tabColor rgb="FF00E676"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="B1:Q38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28:G28"/>
+      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -527,23 +573,23 @@
       </c>
       <c r="M5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>10679</v>
+        <v>5082</v>
       </c>
       <c r="N5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>11122</v>
+        <v>13211</v>
       </c>
       <c r="O5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>1854</v>
+        <v>29914</v>
       </c>
       <c r="P5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>4135</v>
+        <v>28291</v>
       </c>
       <c r="Q5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>4073</v>
+        <v>17390</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -571,34 +617,34 @@
       </c>
       <c r="J6" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K6" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L6" s="12" t="str">
         <f aca="false">I6&amp;"."&amp;J6&amp;"."&amp;K6</f>
-        <v>4.5.2022</v>
+        <v>4.4.2022</v>
       </c>
       <c r="M6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>24645</v>
+        <v>8789</v>
       </c>
       <c r="N6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>3865</v>
+        <v>17229</v>
       </c>
       <c r="O6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>21736</v>
+        <v>7742</v>
       </c>
       <c r="P6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>27148</v>
+        <v>6376</v>
       </c>
       <c r="Q6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>17640</v>
+        <v>25466</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -622,38 +668,38 @@
       </c>
       <c r="I7" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J7" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K7" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L7" s="12" t="str">
         <f aca="false">I7&amp;"."&amp;J7&amp;"."&amp;K7</f>
-        <v>4.7.2022</v>
+        <v>7.3.2022</v>
       </c>
       <c r="M7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>22355</v>
+        <v>444</v>
       </c>
       <c r="N7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>8254</v>
+        <v>28419</v>
       </c>
       <c r="O7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>23004</v>
+        <v>14025</v>
       </c>
       <c r="P7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>18795</v>
+        <v>3622</v>
       </c>
       <c r="Q7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>2161</v>
+        <v>12801</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -677,38 +723,38 @@
       </c>
       <c r="I8" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J8" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K8" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L8" s="12" t="str">
         <f aca="false">I8&amp;"."&amp;J8&amp;"."&amp;K8</f>
-        <v>10.1.2022</v>
+        <v>9.10.2022</v>
       </c>
       <c r="M8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>28129</v>
+        <v>23847</v>
       </c>
       <c r="N8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>28247</v>
+        <v>8808</v>
       </c>
       <c r="O8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>9471</v>
+        <v>29251</v>
       </c>
       <c r="P8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>11840</v>
+        <v>21322</v>
       </c>
       <c r="Q8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>12160</v>
+        <v>8762</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -732,38 +778,38 @@
       </c>
       <c r="I9" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J9" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K9" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L9" s="12" t="str">
         <f aca="false">I9&amp;"."&amp;J9&amp;"."&amp;K9</f>
-        <v>8.6.2022</v>
+        <v>10.1.2022</v>
       </c>
       <c r="M9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>8306</v>
+        <v>29800</v>
       </c>
       <c r="N9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>12503</v>
+        <v>8566</v>
       </c>
       <c r="O9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>11301</v>
+        <v>2578</v>
       </c>
       <c r="P9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>26208</v>
+        <v>25530</v>
       </c>
       <c r="Q9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>2496</v>
+        <v>3170</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -787,38 +833,38 @@
       </c>
       <c r="I10" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J10" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K10" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L10" s="12" t="str">
         <f aca="false">I10&amp;"."&amp;J10&amp;"."&amp;K10</f>
-        <v>5.3.2022</v>
+        <v>7.8.2022</v>
       </c>
       <c r="M10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>2094</v>
+        <v>2320</v>
       </c>
       <c r="N10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>4135</v>
+        <v>26542</v>
       </c>
       <c r="O10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>6287</v>
+        <v>18502</v>
       </c>
       <c r="P10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>26125</v>
+        <v>27343</v>
       </c>
       <c r="Q10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>14182</v>
+        <v>28332</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -842,7 +888,7 @@
       </c>
       <c r="I11" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J11" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
@@ -853,27 +899,27 @@
       </c>
       <c r="L11" s="12" t="str">
         <f aca="false">I11&amp;"."&amp;J11&amp;"."&amp;K11</f>
-        <v>4.6.2022</v>
+        <v>5.6.2022</v>
       </c>
       <c r="M11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>11394</v>
+        <v>3624</v>
       </c>
       <c r="N11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>20221</v>
+        <v>3210</v>
       </c>
       <c r="O11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>23739</v>
+        <v>22720</v>
       </c>
       <c r="P11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>14737</v>
+        <v>11010</v>
       </c>
       <c r="Q11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>24905</v>
+        <v>21735</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1026,38 +1072,38 @@
       </c>
       <c r="I17" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J17" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="K17" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L17" s="12" t="str">
         <f aca="false">I17&amp;"."&amp;J17&amp;"."&amp;K17</f>
-        <v>2.1.2022</v>
+        <v>5.12.2022</v>
       </c>
       <c r="M17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>15612</v>
+        <v>20376</v>
       </c>
       <c r="N17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>16065</v>
+        <v>24437</v>
       </c>
       <c r="O17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>24580</v>
+        <v>19104</v>
       </c>
       <c r="P17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>17939</v>
+        <v>24484</v>
       </c>
       <c r="Q17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>13255</v>
+        <v>6765</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1085,34 +1131,34 @@
       </c>
       <c r="J18" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K18" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L18" s="12" t="str">
         <f aca="false">I18&amp;"."&amp;J18&amp;"."&amp;K18</f>
-        <v>8.3.2022</v>
+        <v>8.8.2022</v>
       </c>
       <c r="M18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>2252</v>
+        <v>19935</v>
       </c>
       <c r="N18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>13250</v>
+        <v>19073</v>
       </c>
       <c r="O18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>11748</v>
+        <v>7550</v>
       </c>
       <c r="P18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>12422</v>
+        <v>27251</v>
       </c>
       <c r="Q18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>16331</v>
+        <v>3481</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1136,38 +1182,38 @@
       </c>
       <c r="I19" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J19" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="K19" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L19" s="12" t="str">
         <f aca="false">I19&amp;"."&amp;J19&amp;"."&amp;K19</f>
-        <v>2.9.2022</v>
+        <v>10.2.2022</v>
       </c>
       <c r="M19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>2169</v>
+        <v>13075</v>
       </c>
       <c r="N19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>20502</v>
+        <v>28980</v>
       </c>
       <c r="O19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>1134</v>
+        <v>23750</v>
       </c>
       <c r="P19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>14961</v>
+        <v>22149</v>
       </c>
       <c r="Q19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>28600</v>
+        <v>9629</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1191,38 +1237,38 @@
       </c>
       <c r="I20" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J20" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K20" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L20" s="12" t="str">
         <f aca="false">I20&amp;"."&amp;J20&amp;"."&amp;K20</f>
-        <v>1.11.2022</v>
+        <v>5.10.2022</v>
       </c>
       <c r="M20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>15244</v>
+        <v>22555</v>
       </c>
       <c r="N20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>15591</v>
+        <v>14535</v>
       </c>
       <c r="O20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>10451</v>
+        <v>23431</v>
       </c>
       <c r="P20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>22863</v>
+        <v>29271</v>
       </c>
       <c r="Q20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>17721</v>
+        <v>16825</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1246,38 +1292,38 @@
       </c>
       <c r="I21" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="J21" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="K21" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L21" s="12" t="str">
         <f aca="false">I21&amp;"."&amp;J21&amp;"."&amp;K21</f>
-        <v>4.2.2022</v>
+        <v>9.11.2022</v>
       </c>
       <c r="M21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>6975</v>
+        <v>19250</v>
       </c>
       <c r="N21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>24424</v>
+        <v>14303</v>
       </c>
       <c r="O21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>9448</v>
+        <v>19925</v>
       </c>
       <c r="P21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>16868</v>
+        <v>8551</v>
       </c>
       <c r="Q21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>5818</v>
+        <v>8352</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1301,38 +1347,38 @@
       </c>
       <c r="I22" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J22" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="K22" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L22" s="12" t="str">
         <f aca="false">I22&amp;"."&amp;J22&amp;"."&amp;K22</f>
-        <v>7.12.2022</v>
+        <v>9.9.2022</v>
       </c>
       <c r="M22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>18737</v>
+        <v>14508</v>
       </c>
       <c r="N22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>287</v>
+        <v>4763</v>
       </c>
       <c r="O22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>9335</v>
+        <v>5603</v>
       </c>
       <c r="P22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>25869</v>
+        <v>6272</v>
       </c>
       <c r="Q22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>5946</v>
+        <v>13920</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1356,38 +1402,38 @@
       </c>
       <c r="I23" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="J23" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="K23" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L23" s="12" t="str">
         <f aca="false">I23&amp;"."&amp;J23&amp;"."&amp;K23</f>
-        <v>4.10.2022</v>
+        <v>9.2.2022</v>
       </c>
       <c r="M23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>16932</v>
+        <v>9606</v>
       </c>
       <c r="N23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>123</v>
+        <v>10534</v>
       </c>
       <c r="O23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>9958</v>
+        <v>17788</v>
       </c>
       <c r="P23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>17545</v>
+        <v>4872</v>
       </c>
       <c r="Q23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>18235</v>
+        <v>2425</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1540,38 +1586,38 @@
       </c>
       <c r="I29" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J29" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="K29" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L29" s="12" t="str">
         <f aca="false">I29&amp;"."&amp;J29&amp;"."&amp;K29</f>
-        <v>3.12.2022</v>
+        <v>1.3.2022</v>
       </c>
       <c r="M29" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>3656</v>
+        <v>8561</v>
       </c>
       <c r="N29" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>14428</v>
+        <v>8547</v>
       </c>
       <c r="O29" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>29056</v>
+        <v>18433</v>
       </c>
       <c r="P29" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>15381</v>
+        <v>20233</v>
       </c>
       <c r="Q29" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>17841</v>
+        <v>2754</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1595,38 +1641,38 @@
       </c>
       <c r="I30" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J30" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K30" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L30" s="12" t="str">
         <f aca="false">I30&amp;"."&amp;J30&amp;"."&amp;K30</f>
-        <v>3.1.2022</v>
+        <v>1.2.2022</v>
       </c>
       <c r="M30" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>8343</v>
+        <v>23080</v>
       </c>
       <c r="N30" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>3866</v>
+        <v>10138</v>
       </c>
       <c r="O30" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>5095</v>
+        <v>10391</v>
       </c>
       <c r="P30" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>16218</v>
+        <v>6619</v>
       </c>
       <c r="Q30" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>19311</v>
+        <v>4432</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1650,38 +1696,38 @@
       </c>
       <c r="I31" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="J31" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="K31" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L31" s="12" t="str">
         <f aca="false">I31&amp;"."&amp;J31&amp;"."&amp;K31</f>
-        <v>3.2.2022</v>
+        <v>7.10.2022</v>
       </c>
       <c r="M31" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>28480</v>
+        <v>25854</v>
       </c>
       <c r="N31" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>8987</v>
+        <v>7670</v>
       </c>
       <c r="O31" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>3493</v>
+        <v>20412</v>
       </c>
       <c r="P31" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>12818</v>
+        <v>24301</v>
       </c>
       <c r="Q31" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>21949</v>
+        <v>19479</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1705,38 +1751,38 @@
       </c>
       <c r="I32" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="J32" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="K32" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L32" s="12" t="str">
         <f aca="false">I32&amp;"."&amp;J32&amp;"."&amp;K32</f>
-        <v>5.11.2022</v>
+        <v>9.1.2022</v>
       </c>
       <c r="M32" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>17486</v>
+        <v>1470</v>
       </c>
       <c r="N32" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>6015</v>
+        <v>19892</v>
       </c>
       <c r="O32" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>19297</v>
+        <v>12974</v>
       </c>
       <c r="P32" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>10734</v>
+        <v>4074</v>
       </c>
       <c r="Q32" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>15058</v>
+        <v>23012</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1760,38 +1806,38 @@
       </c>
       <c r="I33" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="J33" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K33" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L33" s="12" t="str">
         <f aca="false">I33&amp;"."&amp;J33&amp;"."&amp;K33</f>
-        <v>10.10.2022</v>
+        <v>1.9.2022</v>
       </c>
       <c r="M33" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>3134</v>
+        <v>4596</v>
       </c>
       <c r="N33" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>17688</v>
+        <v>8752</v>
       </c>
       <c r="O33" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>19272</v>
+        <v>27236</v>
       </c>
       <c r="P33" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>23641</v>
+        <v>20215</v>
       </c>
       <c r="Q33" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>4401</v>
+        <v>6520</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1815,7 +1861,7 @@
       </c>
       <c r="I34" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="J34" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
@@ -1826,27 +1872,27 @@
       </c>
       <c r="L34" s="12" t="str">
         <f aca="false">I34&amp;"."&amp;J34&amp;"."&amp;K34</f>
-        <v>10.4.2022</v>
+        <v>7.4.2022</v>
       </c>
       <c r="M34" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>27663</v>
+        <v>23054</v>
       </c>
       <c r="N34" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>13487</v>
+        <v>5797</v>
       </c>
       <c r="O34" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>25888</v>
+        <v>29749</v>
       </c>
       <c r="P34" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>5133</v>
+        <v>21965</v>
       </c>
       <c r="Q34" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>350</v>
+        <v>28032</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1870,38 +1916,38 @@
       </c>
       <c r="I35" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J35" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="K35" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L35" s="12" t="str">
         <f aca="false">I35&amp;"."&amp;J35&amp;"."&amp;K35</f>
-        <v>6.11.2022</v>
+        <v>2.5.2022</v>
       </c>
       <c r="M35" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>13880</v>
+        <v>21586</v>
       </c>
       <c r="N35" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>18091</v>
+        <v>3257</v>
       </c>
       <c r="O35" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>16367</v>
+        <v>11438</v>
       </c>
       <c r="P35" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>3146</v>
+        <v>19749</v>
       </c>
       <c r="Q35" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>19698</v>
+        <v>28267</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2035,52 +2081,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C28:G28 A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C28:G28 A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -2089,7 +2089,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C28:G28 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
birlestir fonksiyonu da calisiyor.
eklenecek yeni ozellikler incelenecek...
</commit_message>
<xml_diff>
--- a/D3.xlsx
+++ b/D3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sayfa2" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="Sayfa3" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="syf1" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="syf1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sayfa2" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Sayfa3" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="Sayfa4" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -418,52 +418,6 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
     <tabColor rgb="FF00E676"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -558,38 +512,38 @@
       </c>
       <c r="I5" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J5" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="K5" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L5" s="12" t="str">
         <f aca="false">I5&amp;"."&amp;J5&amp;"."&amp;K5</f>
-        <v>7.2.2022</v>
+        <v>9.9.2022</v>
       </c>
       <c r="M5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>5082</v>
+        <v>22322</v>
       </c>
       <c r="N5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>13211</v>
+        <v>14076</v>
       </c>
       <c r="O5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>29914</v>
+        <v>2411</v>
       </c>
       <c r="P5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>28291</v>
+        <v>8669</v>
       </c>
       <c r="Q5" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>17390</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -613,38 +567,38 @@
       </c>
       <c r="I6" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J6" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="K6" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L6" s="12" t="str">
         <f aca="false">I6&amp;"."&amp;J6&amp;"."&amp;K6</f>
-        <v>4.4.2022</v>
+        <v>1.9.2022</v>
       </c>
       <c r="M6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>8789</v>
+        <v>20681</v>
       </c>
       <c r="N6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>17229</v>
+        <v>10302</v>
       </c>
       <c r="O6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>7742</v>
+        <v>2131</v>
       </c>
       <c r="P6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>6376</v>
+        <v>14478</v>
       </c>
       <c r="Q6" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>25466</v>
+        <v>18808</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -668,38 +622,38 @@
       </c>
       <c r="I7" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J7" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="K7" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L7" s="12" t="str">
         <f aca="false">I7&amp;"."&amp;J7&amp;"."&amp;K7</f>
-        <v>7.3.2022</v>
+        <v>4.12.2022</v>
       </c>
       <c r="M7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>444</v>
+        <v>24529</v>
       </c>
       <c r="N7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>28419</v>
+        <v>9017</v>
       </c>
       <c r="O7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>14025</v>
+        <v>10732</v>
       </c>
       <c r="P7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>3622</v>
+        <v>3836</v>
       </c>
       <c r="Q7" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>12801</v>
+        <v>27319</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -723,38 +677,38 @@
       </c>
       <c r="I8" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J8" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="K8" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L8" s="12" t="str">
         <f aca="false">I8&amp;"."&amp;J8&amp;"."&amp;K8</f>
-        <v>9.10.2022</v>
+        <v>10.8.2022</v>
       </c>
       <c r="M8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>23847</v>
+        <v>16361</v>
       </c>
       <c r="N8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>8808</v>
+        <v>19548</v>
       </c>
       <c r="O8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>29251</v>
+        <v>21341</v>
       </c>
       <c r="P8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>21322</v>
+        <v>20558</v>
       </c>
       <c r="Q8" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>8762</v>
+        <v>11943</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -778,38 +732,38 @@
       </c>
       <c r="I9" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="J9" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="K9" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L9" s="12" t="str">
         <f aca="false">I9&amp;"."&amp;J9&amp;"."&amp;K9</f>
-        <v>10.1.2022</v>
+        <v>1.12.2022</v>
       </c>
       <c r="M9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>29800</v>
+        <v>26721</v>
       </c>
       <c r="N9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>8566</v>
+        <v>22950</v>
       </c>
       <c r="O9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>2578</v>
+        <v>7429</v>
       </c>
       <c r="P9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>25530</v>
+        <v>10953</v>
       </c>
       <c r="Q9" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>3170</v>
+        <v>5862</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -833,38 +787,38 @@
       </c>
       <c r="I10" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J10" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="K10" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L10" s="12" t="str">
         <f aca="false">I10&amp;"."&amp;J10&amp;"."&amp;K10</f>
-        <v>7.8.2022</v>
+        <v>5.12.2022</v>
       </c>
       <c r="M10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>2320</v>
+        <v>16264</v>
       </c>
       <c r="N10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>26542</v>
+        <v>26399</v>
       </c>
       <c r="O10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>18502</v>
+        <v>11294</v>
       </c>
       <c r="P10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>27343</v>
+        <v>14686</v>
       </c>
       <c r="Q10" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>28332</v>
+        <v>5078</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -888,38 +842,38 @@
       </c>
       <c r="I11" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J11" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K11" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L11" s="12" t="str">
         <f aca="false">I11&amp;"."&amp;J11&amp;"."&amp;K11</f>
-        <v>5.6.2022</v>
+        <v>8.2.2022</v>
       </c>
       <c r="M11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>3624</v>
+        <v>641</v>
       </c>
       <c r="N11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>3210</v>
+        <v>21686</v>
       </c>
       <c r="O11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>22720</v>
+        <v>2313</v>
       </c>
       <c r="P11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>11010</v>
+        <v>7967</v>
       </c>
       <c r="Q11" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>21735</v>
+        <v>13923</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1072,38 +1026,38 @@
       </c>
       <c r="I17" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J17" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="K17" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L17" s="12" t="str">
         <f aca="false">I17&amp;"."&amp;J17&amp;"."&amp;K17</f>
-        <v>5.12.2022</v>
+        <v>7.4.2022</v>
       </c>
       <c r="M17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>20376</v>
+        <v>26434</v>
       </c>
       <c r="N17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>24437</v>
+        <v>20326</v>
       </c>
       <c r="O17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>19104</v>
+        <v>3278</v>
       </c>
       <c r="P17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>24484</v>
+        <v>11286</v>
       </c>
       <c r="Q17" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>6765</v>
+        <v>16766</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1131,34 +1085,34 @@
       </c>
       <c r="J18" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="K18" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L18" s="12" t="str">
         <f aca="false">I18&amp;"."&amp;J18&amp;"."&amp;K18</f>
-        <v>8.8.2022</v>
+        <v>8.2.2022</v>
       </c>
       <c r="M18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>19935</v>
+        <v>6110</v>
       </c>
       <c r="N18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>19073</v>
+        <v>17245</v>
       </c>
       <c r="O18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>7550</v>
+        <v>2854</v>
       </c>
       <c r="P18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>27251</v>
+        <v>20372</v>
       </c>
       <c r="Q18" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>3481</v>
+        <v>4798</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1186,34 +1140,34 @@
       </c>
       <c r="J19" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="K19" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L19" s="12" t="str">
         <f aca="false">I19&amp;"."&amp;J19&amp;"."&amp;K19</f>
-        <v>10.2.2022</v>
+        <v>10.8.2022</v>
       </c>
       <c r="M19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>13075</v>
+        <v>9230</v>
       </c>
       <c r="N19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>28980</v>
+        <v>21658</v>
       </c>
       <c r="O19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>23750</v>
+        <v>16737</v>
       </c>
       <c r="P19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>22149</v>
+        <v>13925</v>
       </c>
       <c r="Q19" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>9629</v>
+        <v>8203</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1237,7 +1191,7 @@
       </c>
       <c r="I20" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J20" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
@@ -1248,27 +1202,27 @@
       </c>
       <c r="L20" s="12" t="str">
         <f aca="false">I20&amp;"."&amp;J20&amp;"."&amp;K20</f>
-        <v>5.10.2022</v>
+        <v>7.10.2022</v>
       </c>
       <c r="M20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>22555</v>
+        <v>12518</v>
       </c>
       <c r="N20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>14535</v>
+        <v>19758</v>
       </c>
       <c r="O20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>23431</v>
+        <v>485</v>
       </c>
       <c r="P20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>29271</v>
+        <v>7904</v>
       </c>
       <c r="Q20" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>16825</v>
+        <v>12966</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1292,38 +1246,38 @@
       </c>
       <c r="I21" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J21" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K21" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L21" s="12" t="str">
         <f aca="false">I21&amp;"."&amp;J21&amp;"."&amp;K21</f>
-        <v>9.11.2022</v>
+        <v>5.10.2022</v>
       </c>
       <c r="M21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>19250</v>
+        <v>11260</v>
       </c>
       <c r="N21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>14303</v>
+        <v>11754</v>
       </c>
       <c r="O21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>19925</v>
+        <v>24944</v>
       </c>
       <c r="P21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>8551</v>
+        <v>25005</v>
       </c>
       <c r="Q21" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>8352</v>
+        <v>28292</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1351,34 +1305,34 @@
       </c>
       <c r="J22" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K22" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L22" s="12" t="str">
         <f aca="false">I22&amp;"."&amp;J22&amp;"."&amp;K22</f>
-        <v>9.9.2022</v>
+        <v>9.8.2022</v>
       </c>
       <c r="M22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>14508</v>
+        <v>12948</v>
       </c>
       <c r="N22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>4763</v>
+        <v>13523</v>
       </c>
       <c r="O22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>5603</v>
+        <v>2021</v>
       </c>
       <c r="P22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>6272</v>
+        <v>14217</v>
       </c>
       <c r="Q22" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>13920</v>
+        <v>7996</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1402,38 +1356,38 @@
       </c>
       <c r="I23" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="J23" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K23" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L23" s="12" t="str">
         <f aca="false">I23&amp;"."&amp;J23&amp;"."&amp;K23</f>
-        <v>9.2.2022</v>
+        <v>2.3.2022</v>
       </c>
       <c r="M23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>9606</v>
+        <v>21623</v>
       </c>
       <c r="N23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>10534</v>
+        <v>18174</v>
       </c>
       <c r="O23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>17788</v>
+        <v>19010</v>
       </c>
       <c r="P23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>4872</v>
+        <v>10099</v>
       </c>
       <c r="Q23" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>2425</v>
+        <v>18216</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1586,38 +1540,38 @@
       </c>
       <c r="I29" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="J29" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="K29" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L29" s="12" t="str">
         <f aca="false">I29&amp;"."&amp;J29&amp;"."&amp;K29</f>
-        <v>1.3.2022</v>
+        <v>9.11.2022</v>
       </c>
       <c r="M29" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>8561</v>
+        <v>26493</v>
       </c>
       <c r="N29" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>8547</v>
+        <v>14543</v>
       </c>
       <c r="O29" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>18433</v>
+        <v>22826</v>
       </c>
       <c r="P29" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>20233</v>
+        <v>7553</v>
       </c>
       <c r="Q29" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>2754</v>
+        <v>10798</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1641,38 +1595,38 @@
       </c>
       <c r="I30" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J30" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="K30" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L30" s="12" t="str">
         <f aca="false">I30&amp;"."&amp;J30&amp;"."&amp;K30</f>
-        <v>1.2.2022</v>
+        <v>7.7.2022</v>
       </c>
       <c r="M30" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>23080</v>
+        <v>14355</v>
       </c>
       <c r="N30" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>10138</v>
+        <v>19118</v>
       </c>
       <c r="O30" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>10391</v>
+        <v>27660</v>
       </c>
       <c r="P30" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>6619</v>
+        <v>12566</v>
       </c>
       <c r="Q30" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>4432</v>
+        <v>11351</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1696,38 +1650,38 @@
       </c>
       <c r="I31" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J31" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="K31" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L31" s="12" t="str">
         <f aca="false">I31&amp;"."&amp;J31&amp;"."&amp;K31</f>
-        <v>7.10.2022</v>
+        <v>5.2.2022</v>
       </c>
       <c r="M31" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>25854</v>
+        <v>14364</v>
       </c>
       <c r="N31" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>7670</v>
+        <v>1894</v>
       </c>
       <c r="O31" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>20412</v>
+        <v>16767</v>
       </c>
       <c r="P31" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>24301</v>
+        <v>25478</v>
       </c>
       <c r="Q31" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>19479</v>
+        <v>23104</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1751,38 +1705,38 @@
       </c>
       <c r="I32" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J32" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="K32" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L32" s="12" t="str">
         <f aca="false">I32&amp;"."&amp;J32&amp;"."&amp;K32</f>
-        <v>9.1.2022</v>
+        <v>10.12.2022</v>
       </c>
       <c r="M32" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>1470</v>
+        <v>16125</v>
       </c>
       <c r="N32" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>19892</v>
+        <v>410</v>
       </c>
       <c r="O32" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>12974</v>
+        <v>24967</v>
       </c>
       <c r="P32" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>4074</v>
+        <v>25470</v>
       </c>
       <c r="Q32" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>23012</v>
+        <v>23014</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1806,38 +1760,38 @@
       </c>
       <c r="I33" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J33" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="K33" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L33" s="12" t="str">
         <f aca="false">I33&amp;"."&amp;J33&amp;"."&amp;K33</f>
-        <v>1.9.2022</v>
+        <v>2.2.2022</v>
       </c>
       <c r="M33" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>4596</v>
+        <v>29413</v>
       </c>
       <c r="N33" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>8752</v>
+        <v>6414</v>
       </c>
       <c r="O33" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>27236</v>
+        <v>8405</v>
       </c>
       <c r="P33" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>20215</v>
+        <v>15935</v>
       </c>
       <c r="Q33" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>6520</v>
+        <v>16677</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1865,34 +1819,34 @@
       </c>
       <c r="J34" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="K34" s="12" t="n">
         <v>2022</v>
       </c>
       <c r="L34" s="12" t="str">
         <f aca="false">I34&amp;"."&amp;J34&amp;"."&amp;K34</f>
-        <v>7.4.2022</v>
+        <v>7.11.2022</v>
       </c>
       <c r="M34" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>23054</v>
+        <v>14289</v>
       </c>
       <c r="N34" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>5797</v>
+        <v>14158</v>
       </c>
       <c r="O34" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>29749</v>
+        <v>17092</v>
       </c>
       <c r="P34" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>21965</v>
+        <v>18977</v>
       </c>
       <c r="Q34" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>28032</v>
+        <v>9096</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1916,7 +1870,7 @@
       </c>
       <c r="I35" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,10)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="J35" s="12" t="n">
         <f aca="false">RANDBETWEEN(1,12)</f>
@@ -1927,27 +1881,27 @@
       </c>
       <c r="L35" s="12" t="str">
         <f aca="false">I35&amp;"."&amp;J35&amp;"."&amp;K35</f>
-        <v>2.5.2022</v>
+        <v>7.5.2022</v>
       </c>
       <c r="M35" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>21586</v>
+        <v>11508</v>
       </c>
       <c r="N35" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>3257</v>
+        <v>10744</v>
       </c>
       <c r="O35" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>11438</v>
+        <v>6348</v>
       </c>
       <c r="P35" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>19749</v>
+        <v>3902</v>
       </c>
       <c r="Q35" s="13" t="n">
         <f aca="false">RANDBETWEEN(100,30000)</f>
-        <v>28267</v>
+        <v>22815</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2081,6 +2035,52 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Sayfa &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">

</xml_diff>